<commit_message>
SIQ Document Reviewed and some comments added .
</commit_message>
<xml_diff>
--- a/Project V 1.1.xlsx
+++ b/Project V 1.1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hossa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProjectManagementProject\Foodies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25714" windowHeight="13723"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25716" windowHeight="13728"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Revision_History" sheetId="3" r:id="rId1"/>
+    <sheet name="SIQ_V1" sheetId="1" r:id="rId2"/>
+    <sheet name="PeerReviewNotes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -290,14 +291,118 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Approved by</t>
+    <t>SIQ_ID</t>
+  </si>
+  <si>
+    <t>Proposed Solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English/ Franko </t>
+  </si>
+  <si>
+    <t>*Length - Minimum [8] Maximum [10]
+*Accepts Alphanumeric and Special Character.
+ * Must have 2 Capital letters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in question : what are the supported languages ? </t>
+  </si>
+  <si>
+    <t>in question :
+ What is the Characteristics of Strong Password  ?</t>
+  </si>
+  <si>
+    <t>* add Confirm password field 
+*  it's important to be clear about the userID , it must be unique to each user ( not included in db for another user ).
+* Remove make wireframes for registeration form (we'll support this wireframes in design phase ).</t>
+  </si>
+  <si>
+    <t>in question : what's the main content of ….</t>
+  </si>
+  <si>
+    <t>*I think he only mentioned that login will be with UserID
+email will be used in forget password ??
+* clearly mention that userID and password will be text Field as you mentioned that registernow will be link and so on .</t>
+  </si>
+  <si>
+    <t>Do you prefer the existence of alert message that inform the 
+user that the system will access his location ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an alert with yes and no should exist to ask user if 
+it's allowed for the system to acces his location or not </t>
+  </si>
+  <si>
+    <t xml:space="preserve">what are </t>
+  </si>
+  <si>
+    <t>shall the user will be able to register with …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5KM not 5000 km </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes </t>
+  </si>
+  <si>
+    <t>SIQ_11 , SIQ_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replace both questions with this </t>
+  </si>
+  <si>
+    <t>what's the accepted distance between 
+the user and the nearby restaurantsraunts ?</t>
+  </si>
+  <si>
+    <t>How the nearby restaurantsraunts list will be presented ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* restaurantsraunts will be sorted aphabetically.
+* only five restaurantsraunts per page </t>
+  </si>
+  <si>
+    <t>what if No nearby restaurantsraunts found ?</t>
+  </si>
+  <si>
+    <t>display a message "There was no restaurantsaurants found".</t>
+  </si>
+  <si>
+    <t>what if the user want to search 
+in the resulted restaurantsraunts ? Shall he exaclty 
+wirte the restaurantsraunt name of substring of it ?</t>
+  </si>
+  <si>
+    <t>Exact search (write th ecomplete name
+ of the restaurantsraunt as it is )</t>
+  </si>
+  <si>
+    <t>restaurantsraunts</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>28/4/2019</t>
+  </si>
+  <si>
+    <t>Marwa Sheshtawy</t>
+  </si>
+  <si>
+    <t>Hossam Galal</t>
+  </si>
+  <si>
+    <t>Intial SIQ Creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review Dosument , modify some questions and solutions for clarity  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,8 +426,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,8 +455,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -402,11 +528,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -422,6 +592,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,26 +895,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.84375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.23046875" style="1"/>
-    <col min="3" max="3" width="60.15234375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.3046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.23046875" style="1"/>
-    <col min="7" max="7" width="23.3828125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.765625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="1" width="27.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="37" style="12" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" style="1"/>
+    <col min="3" max="3" width="60.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" style="1"/>
+    <col min="7" max="7" width="23.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -735,20 +989,8 @@
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -762,7 +1004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -776,7 +1018,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -790,7 +1032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -804,7 +1046,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -818,7 +1060,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -832,7 +1074,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -846,7 +1088,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -860,7 +1102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -874,7 +1116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -888,7 +1130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -902,7 +1144,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -916,7 +1158,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -930,7 +1172,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -944,7 +1186,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -958,7 +1200,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -972,7 +1214,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -986,7 +1228,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1000,7 +1242,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1018,4 +1260,169 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="54.21875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="104.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="87" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>